<commit_message>
Add Price Entry Table and Provider Dialog
</commit_message>
<xml_diff>
--- a/assets/provider_information.xlsx
+++ b/assets/provider_information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefan/Lokal/Flutter/rag_tco/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5062C701-7567-B54D-9CD7-41B563BE50B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68819FF8-A282-FC41-90C0-4718AF241665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="2760" windowWidth="27840" windowHeight="16740" xr2:uid="{B0654A3F-56E8-B440-A290-FF98AE9EE87D}"/>
+    <workbookView xWindow="39260" yWindow="2280" windowWidth="27840" windowHeight="16740" xr2:uid="{B0654A3F-56E8-B440-A290-FF98AE9EE87D}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Meta</t>
+    <t>Meta Serevice 1</t>
+  </si>
+  <si>
+    <t>Meta Service 2</t>
+  </si>
+  <si>
+    <t>AWS Service 1</t>
+  </si>
+  <si>
+    <t>AWS Service 2</t>
   </si>
 </sst>
 </file>
@@ -411,20 +420,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF7FF2C-6B96-8844-9EA7-07D3B31EAAF5}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1">
         <v>12.3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>8.43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>9.43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Multidimensional Provider Costing Structure and edit functionality
</commit_message>
<xml_diff>
--- a/assets/provider_information.xlsx
+++ b/assets/provider_information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefan/Lokal/Flutter/rag_tco/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68819FF8-A282-FC41-90C0-4718AF241665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC688FBC-70BE-7B4B-8FF0-0D299ABE7DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39260" yWindow="2280" windowWidth="27840" windowHeight="16740" xr2:uid="{B0654A3F-56E8-B440-A290-FF98AE9EE87D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
   <si>
     <t>Meta Serevice 1</t>
   </si>
@@ -48,6 +48,15 @@
   </si>
   <si>
     <t>AWS Service 2</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>1 Mil Calls</t>
   </si>
 </sst>
 </file>
@@ -83,9 +92,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -420,47 +428,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF7FF2C-6B96-8844-9EA7-07D3B31EAAF5}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>12.3</v>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>9.1999999999999993</v>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>8.43</v>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
-        <v>9.43</v>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added multiple component data storage + edit
</commit_message>
<xml_diff>
--- a/assets/provider_information.xlsx
+++ b/assets/provider_information.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefan/Lokal/Flutter/rag_tco/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC688FBC-70BE-7B4B-8FF0-0D299ABE7DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15B6A20-192D-6249-8044-5B431EE81796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39260" yWindow="2280" windowWidth="27840" windowHeight="16740" xr2:uid="{B0654A3F-56E8-B440-A290-FF98AE9EE87D}"/>
   </bookViews>
@@ -36,19 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
-  <si>
-    <t>Meta Serevice 1</t>
-  </si>
-  <si>
-    <t>Meta Service 2</t>
-  </si>
-  <si>
-    <t>AWS Service 1</t>
-  </si>
-  <si>
-    <t>AWS Service 2</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>Input</t>
   </si>
@@ -56,7 +44,13 @@
     <t>Output</t>
   </si>
   <si>
-    <t>1 Mil Calls</t>
+    <t>GPT-4o</t>
+  </si>
+  <si>
+    <t>GPT-4o Batched</t>
+  </si>
+  <si>
+    <t>Token</t>
   </si>
 </sst>
 </file>
@@ -428,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF7FF2C-6B96-8844-9EA7-07D3B31EAAF5}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -439,96 +433,62 @@
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1">
+        <v>5</v>
+      </c>
+      <c r="D1">
+        <v>1000000</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="C1">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1">
+        <v>15</v>
+      </c>
+      <c r="H1">
+        <v>1000000</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>2.5</v>
+      </c>
+      <c r="D2">
+        <v>1000000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2">
         <v>5</v>
       </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="H2">
+        <v>1000000</v>
+      </c>
+      <c r="I2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Multiple UnitTypes, Service Entry Dialog Rebuilded
</commit_message>
<xml_diff>
--- a/assets/provider_information.xlsx
+++ b/assets/provider_information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefan/Lokal/Flutter/rag_tco/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15B6A20-192D-6249-8044-5B431EE81796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13634730-221A-0F47-94F0-047E0CDDF5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39260" yWindow="2280" windowWidth="27840" windowHeight="16740" xr2:uid="{B0654A3F-56E8-B440-A290-FF98AE9EE87D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="24">
   <si>
     <t>Input</t>
   </si>
@@ -47,20 +47,84 @@
     <t>GPT-4o</t>
   </si>
   <si>
-    <t>GPT-4o Batched</t>
-  </si>
-  <si>
     <t>Token</t>
+  </si>
+  <si>
+    <t>GPT-4o mini</t>
+  </si>
+  <si>
+    <t>GPT-4o mini Batch</t>
+  </si>
+  <si>
+    <t>GPT-4o Batch</t>
+  </si>
+  <si>
+    <t>GPT-3.5 Turbo</t>
+  </si>
+  <si>
+    <t>GPT-3.5 Turbo Batch</t>
+  </si>
+  <si>
+    <t>GPT-3.5 Turbo-Instruct</t>
+  </si>
+  <si>
+    <t>GPT-3.5 Turbo-Instruct Batch</t>
+  </si>
+  <si>
+    <t>Gemini 1.0 Pro</t>
+  </si>
+  <si>
+    <t>Picture Input</t>
+  </si>
+  <si>
+    <t>Picture</t>
+  </si>
+  <si>
+    <t>Video Input</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>Text Input</t>
+  </si>
+  <si>
+    <t>Characters</t>
+  </si>
+  <si>
+    <t>Audio Input</t>
+  </si>
+  <si>
+    <t>Gemini 1.5 Pro (=&lt; 128.000 Context Window)</t>
+  </si>
+  <si>
+    <t>Gemini 1.5 Pro (&gt; 128.000 Context Window)</t>
+  </si>
+  <si>
+    <t>Gemini 1.5 Flash (=&lt; 128.000 Context Window)</t>
+  </si>
+  <si>
+    <t>Gemini 1.5 Flash (&gt; 128.000 Context Window)</t>
+  </si>
+  <si>
+    <t>Text Output</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -86,8 +150,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -422,18 +487,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBF7FF2C-6B96-8844-9EA7-07D3B31EAAF5}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="39.5" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -447,7 +513,7 @@
         <v>1000000</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -459,12 +525,12 @@
         <v>1000000</v>
       </c>
       <c r="I1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -476,7 +542,7 @@
         <v>1000000</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>
@@ -488,7 +554,494 @@
         <v>1000000</v>
       </c>
       <c r="I2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0.15</v>
+      </c>
+      <c r="D3">
+        <v>1000000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0.6</v>
+      </c>
+      <c r="H3">
+        <v>1000000</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0.08</v>
+      </c>
+      <c r="D4">
+        <v>1000000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0.3</v>
+      </c>
+      <c r="H4">
+        <v>1000000</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0.5</v>
+      </c>
+      <c r="D5">
+        <v>1000000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1.5</v>
+      </c>
+      <c r="H5">
+        <v>1000000</v>
+      </c>
+      <c r="I5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0.25</v>
+      </c>
+      <c r="D6">
+        <v>1000000</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>0.75</v>
+      </c>
+      <c r="H6">
+        <v>1000000</v>
+      </c>
+      <c r="I6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1.5</v>
+      </c>
+      <c r="D7">
+        <v>1000000</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>1000000</v>
+      </c>
+      <c r="I7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0.75</v>
+      </c>
+      <c r="D8">
+        <v>1000000</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1000000</v>
+      </c>
+      <c r="I8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>1.315E-4</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>1.315E-4</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9">
+        <v>1.25E-4</v>
+      </c>
+      <c r="L9">
+        <v>1000</v>
+      </c>
+      <c r="M9" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" t="s">
+        <v>18</v>
+      </c>
+      <c r="O9">
+        <v>1.2500000000000001E-5</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>15</v>
+      </c>
+      <c r="R9" t="s">
+        <v>23</v>
+      </c>
+      <c r="S9">
+        <v>3.7500000000000001E-4</v>
+      </c>
+      <c r="T9">
+        <v>1000</v>
+      </c>
+      <c r="U9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2.63E-4</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2.63E-4</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10" s="1">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O10" s="1">
+        <v>2.5000000000000001E-5</v>
+      </c>
+      <c r="P10" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R10" t="s">
+        <v>23</v>
+      </c>
+      <c r="S10">
+        <v>7.5000000000000002E-4</v>
+      </c>
+      <c r="T10">
+        <v>1000</v>
+      </c>
+      <c r="U10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1.315E-3</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1.315E-3</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1.25E-3</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O11" s="1">
+        <v>1.25E-4</v>
+      </c>
+      <c r="P11" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R11" t="s">
+        <v>23</v>
+      </c>
+      <c r="S11">
+        <v>3.7499999999999999E-3</v>
+      </c>
+      <c r="T11">
+        <v>1000</v>
+      </c>
+      <c r="U11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2.63E-3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="1">
+        <v>2.63E-3</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O12" s="1">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="P12" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R12" t="s">
+        <v>23</v>
+      </c>
+      <c r="S12">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="T12">
+        <v>1000</v>
+      </c>
+      <c r="U12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1.25E-4</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1000</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O13" s="1">
+        <v>3.7500000000000001E-4</v>
+      </c>
+      <c r="P13" s="1">
+        <v>1000</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>